<commit_message>
added human readable metadata
</commit_message>
<xml_diff>
--- a/deploy/nc-water-supply/data/pcp/ncsu_api_locations.xlsx
+++ b/deploy/nc-water-supply/data/pcp/ncsu_api_locations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lap19\Documents\Internet of Water\Pilots\NC\NC Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lap19\Documents\GitHub\TriangleWaterSupplyDashboard\deploy\nc-water-supply\data\pcp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="406">
   <si>
     <t>B Everett Jordan Dam</t>
   </si>
@@ -1102,12 +1102,6 @@
   </si>
   <si>
     <t>actual start day: 11/1/1871</t>
-  </si>
-  <si>
-    <t>actual start date: 12/1/1870</t>
-  </si>
-  <si>
-    <t>actual start date: 1/1/1887</t>
   </si>
   <si>
     <t>actual start date: 1/15/1892</t>
@@ -1592,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29:L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1603,6 +1597,7 @@
     <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1613,7 +1608,7 @@
         <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>87</v>
@@ -1651,7 +1646,7 @@
         <v>310750</v>
       </c>
       <c r="C2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1686,7 +1681,7 @@
         <v>311429</v>
       </c>
       <c r="C3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -1721,7 +1716,7 @@
         <v>311515</v>
       </c>
       <c r="C4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -1756,7 +1751,7 @@
         <v>311677</v>
       </c>
       <c r="C5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1794,7 +1789,7 @@
         <v>311700</v>
       </c>
       <c r="C6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -1829,7 +1824,7 @@
         <v>311881</v>
       </c>
       <c r="C7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -1864,7 +1859,7 @@
         <v>312500</v>
       </c>
       <c r="C8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -1899,7 +1894,7 @@
         <v>312517</v>
       </c>
       <c r="C9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -1934,7 +1929,7 @@
         <v>313017</v>
       </c>
       <c r="C10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -1972,7 +1967,7 @@
         <v>313555</v>
       </c>
       <c r="C11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -2007,7 +2002,7 @@
         <v>313630</v>
       </c>
       <c r="C12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -2042,7 +2037,7 @@
         <v>313625</v>
       </c>
       <c r="C13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -2077,7 +2072,7 @@
         <v>313919</v>
       </c>
       <c r="C14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -2112,7 +2107,7 @@
         <v>314063</v>
       </c>
       <c r="C15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -2147,7 +2142,7 @@
         <v>314471</v>
       </c>
       <c r="C16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -2174,7 +2169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2182,7 +2177,7 @@
         <v>314987</v>
       </c>
       <c r="C17" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -2209,7 +2204,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2217,7 +2212,7 @@
         <v>315820</v>
       </c>
       <c r="C18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -2244,7 +2239,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2252,7 +2247,7 @@
         <v>315930</v>
       </c>
       <c r="C19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
@@ -2279,7 +2274,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>316122</v>
       </c>
       <c r="C20" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
@@ -2314,7 +2309,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2322,7 +2317,7 @@
         <v>317097</v>
       </c>
       <c r="C21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -2349,7 +2344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2357,7 +2352,7 @@
         <v>316422</v>
       </c>
       <c r="C22" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -2384,7 +2379,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2387,7 @@
         <v>317656</v>
       </c>
       <c r="C23" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -2419,7 +2414,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2427,7 +2422,7 @@
         <v>317924</v>
       </c>
       <c r="C24" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
@@ -2454,7 +2449,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2462,7 +2457,7 @@
         <v>319026</v>
       </c>
       <c r="C25" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
@@ -2489,7 +2484,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -2497,7 +2492,7 @@
         <v>319467</v>
       </c>
       <c r="C26" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
@@ -2524,7 +2519,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -2532,7 +2527,7 @@
         <v>319461</v>
       </c>
       <c r="C27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
@@ -2559,7 +2554,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -2567,7 +2562,7 @@
         <v>319457</v>
       </c>
       <c r="C28" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
@@ -2594,7 +2589,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>99</v>
       </c>
@@ -2602,7 +2597,7 @@
         <v>100</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>131</v>
@@ -2628,12 +2623,11 @@
       <c r="K29" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L29" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>101</v>
       </c>
@@ -2641,7 +2635,7 @@
         <v>102</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>131</v>
@@ -2667,12 +2661,11 @@
       <c r="K30" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L30" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -2680,7 +2673,7 @@
         <v>106</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>131</v>
@@ -2706,12 +2699,11 @@
       <c r="K31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L31" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>109</v>
       </c>
@@ -2719,7 +2711,7 @@
         <v>110</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>131</v>
@@ -2745,12 +2737,11 @@
       <c r="K32" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L32" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>112</v>
       </c>
@@ -2758,7 +2749,7 @@
         <v>113</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>131</v>
@@ -2784,12 +2775,11 @@
       <c r="K33" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L33" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>115</v>
       </c>
@@ -2797,7 +2787,7 @@
         <v>116</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>131</v>
@@ -2823,12 +2813,11 @@
       <c r="K34" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L34" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>117</v>
       </c>
@@ -2836,7 +2825,7 @@
         <v>118</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>131</v>
@@ -2862,12 +2851,11 @@
       <c r="K35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L35" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>120</v>
       </c>
@@ -2875,7 +2863,7 @@
         <v>121</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>131</v>
@@ -2901,12 +2889,11 @@
       <c r="K36" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L36" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>122</v>
       </c>
@@ -2914,7 +2901,7 @@
         <v>123</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>131</v>
@@ -2940,12 +2927,11 @@
       <c r="K37" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L37" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>124</v>
       </c>
@@ -2953,7 +2939,7 @@
         <v>125</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>131</v>
@@ -2979,12 +2965,11 @@
       <c r="K38" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L38" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>126</v>
       </c>
@@ -2992,7 +2977,7 @@
         <v>127</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>131</v>
@@ -3018,12 +3003,11 @@
       <c r="K39" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L39" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>128</v>
       </c>
@@ -3031,7 +3015,7 @@
         <v>129</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>131</v>
@@ -3057,12 +3041,11 @@
       <c r="K40" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L40" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>144</v>
       </c>
@@ -3070,7 +3053,7 @@
         <v>145</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>146</v>
@@ -3096,12 +3079,11 @@
       <c r="K41" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L41" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>149</v>
       </c>
@@ -3109,7 +3091,7 @@
         <v>150</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>146</v>
@@ -3135,12 +3117,11 @@
       <c r="K42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L42" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>152</v>
       </c>
@@ -3148,7 +3129,7 @@
         <v>153</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>146</v>
@@ -3174,12 +3155,11 @@
       <c r="K43" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L43" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>155</v>
       </c>
@@ -3187,7 +3167,7 @@
         <v>156</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>146</v>
@@ -3213,12 +3193,11 @@
       <c r="K44" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L44" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>158</v>
       </c>
@@ -3226,7 +3205,7 @@
         <v>2098197</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>203</v>
@@ -3252,12 +3231,11 @@
       <c r="K45" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L45" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>29</v>
       </c>
@@ -3265,7 +3243,7 @@
         <v>159</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>205</v>
@@ -3291,12 +3269,11 @@
       <c r="K46" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L46" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>160</v>
       </c>
@@ -3304,7 +3281,7 @@
         <v>161</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>207</v>
@@ -3330,12 +3307,11 @@
       <c r="K47" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L47" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>163</v>
       </c>
@@ -3343,7 +3319,7 @@
         <v>164</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>209</v>
@@ -3369,12 +3345,11 @@
       <c r="K48" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L48" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>165</v>
       </c>
@@ -3382,7 +3357,7 @@
         <v>166</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>209</v>
@@ -3409,13 +3384,10 @@
         <v>211</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="M49" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>167</v>
       </c>
@@ -3423,7 +3395,7 @@
         <v>168</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>212</v>
@@ -3449,12 +3421,11 @@
       <c r="K50" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L50" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>169</v>
       </c>
@@ -3462,7 +3433,7 @@
         <v>170</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>212</v>
@@ -3488,12 +3459,11 @@
       <c r="K51" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L51" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>130</v>
       </c>
@@ -3501,7 +3471,7 @@
         <v>171</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>212</v>
@@ -3527,12 +3497,11 @@
       <c r="K52" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L52" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>172</v>
       </c>
@@ -3540,7 +3509,7 @@
         <v>173</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>212</v>
@@ -3566,12 +3535,11 @@
       <c r="K53" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L53" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>175</v>
       </c>
@@ -3579,7 +3547,7 @@
         <v>176</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>212</v>
@@ -3605,12 +3573,11 @@
       <c r="K54" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L54" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>178</v>
       </c>
@@ -3618,7 +3585,7 @@
         <v>179</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>212</v>
@@ -3644,12 +3611,11 @@
       <c r="K55" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L55" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>181</v>
       </c>
@@ -3657,7 +3623,7 @@
         <v>182</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>212</v>
@@ -3683,12 +3649,11 @@
       <c r="K56" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L56" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>183</v>
       </c>
@@ -3696,7 +3661,7 @@
         <v>184</v>
       </c>
       <c r="C57" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D57" t="s">
         <v>220</v>
@@ -3723,7 +3688,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>186</v>
       </c>
@@ -3731,7 +3696,7 @@
         <v>187</v>
       </c>
       <c r="C58" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D58" t="s">
         <v>220</v>
@@ -3758,7 +3723,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>188</v>
       </c>
@@ -3766,7 +3731,7 @@
         <v>189</v>
       </c>
       <c r="C59" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D59" t="s">
         <v>220</v>
@@ -3793,7 +3758,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>191</v>
       </c>
@@ -3801,7 +3766,7 @@
         <v>192</v>
       </c>
       <c r="C60" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D60" t="s">
         <v>220</v>
@@ -3828,7 +3793,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>193</v>
       </c>
@@ -3836,7 +3801,7 @@
         <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D61" t="s">
         <v>220</v>
@@ -3863,7 +3828,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>195</v>
       </c>
@@ -3871,7 +3836,7 @@
         <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D62" t="s">
         <v>220</v>
@@ -3898,7 +3863,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -3906,7 +3871,7 @@
         <v>198</v>
       </c>
       <c r="C63" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D63" t="s">
         <v>220</v>
@@ -3933,7 +3898,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>201</v>
       </c>
@@ -3941,7 +3906,7 @@
         <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D64" t="s">
         <v>220</v>
@@ -3968,7 +3933,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>231</v>
       </c>
@@ -3976,7 +3941,7 @@
         <v>232</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>207</v>
@@ -4002,12 +3967,11 @@
       <c r="K65" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L65" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>234</v>
       </c>
@@ -4015,7 +3979,7 @@
         <v>235</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>209</v>
@@ -4042,13 +4006,10 @@
         <v>237</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="M66" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>238</v>
       </c>
@@ -4056,7 +4017,7 @@
         <v>239</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>212</v>
@@ -4082,12 +4043,11 @@
       <c r="K67" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L67" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>243</v>
       </c>
@@ -4095,7 +4055,7 @@
         <v>244</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>212</v>
@@ -4121,12 +4081,11 @@
       <c r="K68" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L68" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>247</v>
       </c>
@@ -4134,7 +4093,7 @@
         <v>248</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>249</v>
@@ -4160,12 +4119,11 @@
       <c r="K69" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L69" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>251</v>
       </c>
@@ -4173,7 +4131,7 @@
         <v>252</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>249</v>
@@ -4199,12 +4157,11 @@
       <c r="K70" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L70" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>254</v>
       </c>
@@ -4212,7 +4169,7 @@
         <v>255</v>
       </c>
       <c r="C71" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D71" t="s">
         <v>220</v>
@@ -4239,7 +4196,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>259</v>
       </c>
@@ -4247,7 +4204,7 @@
         <v>260</v>
       </c>
       <c r="C72" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D72" t="s">
         <v>220</v>
@@ -4274,7 +4231,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>264</v>
       </c>
@@ -4282,7 +4239,7 @@
         <v>265</v>
       </c>
       <c r="C73" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D73" t="s">
         <v>220</v>
@@ -4309,7 +4266,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>267</v>
       </c>
@@ -4317,7 +4274,7 @@
         <v>268</v>
       </c>
       <c r="C74" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D74" t="s">
         <v>220</v>
@@ -4344,7 +4301,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>272</v>
       </c>
@@ -4352,7 +4309,7 @@
         <v>273</v>
       </c>
       <c r="C75" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D75" t="s">
         <v>220</v>
@@ -4379,7 +4336,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>275</v>
       </c>
@@ -4387,7 +4344,7 @@
         <v>276</v>
       </c>
       <c r="C76" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D76" t="s">
         <v>220</v>
@@ -4414,7 +4371,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -4422,7 +4379,7 @@
         <v>279</v>
       </c>
       <c r="C77" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D77" t="s">
         <v>220</v>
@@ -4449,7 +4406,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>281</v>
       </c>
@@ -4457,7 +4414,7 @@
         <v>282</v>
       </c>
       <c r="C78" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D78" t="s">
         <v>220</v>
@@ -4484,7 +4441,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>284</v>
       </c>
@@ -4492,7 +4449,7 @@
         <v>285</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>146</v>
@@ -4518,12 +4475,11 @@
       <c r="K79" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L79" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>287</v>
       </c>
@@ -4531,7 +4487,7 @@
         <v>288</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>146</v>
@@ -4557,12 +4513,11 @@
       <c r="K80" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L80" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>290</v>
       </c>
@@ -4570,7 +4525,7 @@
         <v>291</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>131</v>
@@ -4596,12 +4551,11 @@
       <c r="K81" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L81" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>294</v>
       </c>
@@ -4609,7 +4563,7 @@
         <v>295</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>131</v>
@@ -4635,12 +4589,11 @@
       <c r="K82" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L82" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>297</v>
       </c>
@@ -4648,7 +4601,7 @@
         <v>298</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>131</v>
@@ -4674,12 +4627,11 @@
       <c r="K83" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L83" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>301</v>
       </c>
@@ -4687,7 +4639,7 @@
         <v>302</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>131</v>
@@ -4713,12 +4665,11 @@
       <c r="K84" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L84" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>306</v>
       </c>
@@ -4726,7 +4677,7 @@
         <v>307</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>131</v>
@@ -4752,12 +4703,11 @@
       <c r="K85" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="L85" s="3"/>
-      <c r="M85" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L85" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>311</v>
       </c>
@@ -4765,7 +4715,7 @@
         <v>312</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>131</v>
@@ -4791,12 +4741,11 @@
       <c r="K86" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L86" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>314</v>
       </c>
@@ -4804,7 +4753,7 @@
         <v>315</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>131</v>
@@ -4830,12 +4779,11 @@
       <c r="K87" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L87" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>64</v>
       </c>
@@ -4843,7 +4791,7 @@
         <v>310212</v>
       </c>
       <c r="C88" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
@@ -4870,7 +4818,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>318</v>
       </c>
@@ -4878,7 +4826,7 @@
         <v>311535</v>
       </c>
       <c r="C89" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D89" t="s">
         <v>1</v>
@@ -4905,7 +4853,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>320</v>
       </c>
@@ -4913,7 +4861,7 @@
         <v>311817</v>
       </c>
       <c r="C90" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
@@ -4940,7 +4888,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>322</v>
       </c>
@@ -4948,7 +4896,7 @@
         <v>311820</v>
       </c>
       <c r="C91" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
@@ -4975,7 +4923,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>231</v>
       </c>
@@ -4983,7 +4931,7 @@
         <v>312993</v>
       </c>
       <c r="C92" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
@@ -5010,7 +4958,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>326</v>
       </c>
@@ -5018,7 +4966,7 @@
         <v>313238</v>
       </c>
       <c r="C93" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
@@ -5045,7 +4993,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>328</v>
       </c>
@@ -5053,7 +5001,7 @@
         <v>313503</v>
       </c>
       <c r="C94" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D94" t="s">
         <v>1</v>
@@ -5080,7 +5028,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>330</v>
       </c>
@@ -5088,7 +5036,7 @@
         <v>314689</v>
       </c>
       <c r="C95" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D95" t="s">
         <v>1</v>
@@ -5115,7 +5063,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>332</v>
       </c>
@@ -5123,7 +5071,7 @@
         <v>316108</v>
       </c>
       <c r="C96" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
@@ -5158,7 +5106,7 @@
         <v>316676</v>
       </c>
       <c r="C97" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D97" t="s">
         <v>1</v>
@@ -5193,7 +5141,7 @@
         <v>317069</v>
       </c>
       <c r="C98" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D98" t="s">
         <v>1</v>
@@ -5228,7 +5176,7 @@
         <v>317079</v>
       </c>
       <c r="C99" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D99" t="s">
         <v>1</v>
@@ -5255,7 +5203,7 @@
         <v>341</v>
       </c>
       <c r="L99" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
@@ -5266,7 +5214,7 @@
         <v>317170</v>
       </c>
       <c r="C100" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D100" t="s">
         <v>1</v>
@@ -5301,7 +5249,7 @@
         <v>317516</v>
       </c>
       <c r="C101" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D101" t="s">
         <v>1</v>
@@ -5328,7 +5276,7 @@
         <v>346</v>
       </c>
       <c r="L101" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
@@ -5339,7 +5287,7 @@
         <v>317994</v>
       </c>
       <c r="C102" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
@@ -5366,7 +5314,7 @@
         <v>347</v>
       </c>
       <c r="L102" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
@@ -5377,7 +5325,7 @@
         <v>318066</v>
       </c>
       <c r="C103" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
@@ -5412,7 +5360,7 @@
         <v>319476</v>
       </c>
       <c r="C104" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D104" t="s">
         <v>1</v>
@@ -5461,268 +5409,268 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C8" t="s">
         <v>377</v>
       </c>
-      <c r="B8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8" t="s">
-        <v>379</v>
-      </c>
       <c r="D8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C9" t="s">
         <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B10" t="s">
+        <v>376</v>
+      </c>
+      <c r="C10" t="s">
         <v>378</v>
       </c>
-      <c r="C10" t="s">
-        <v>380</v>
-      </c>
       <c r="D10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D12" t="s">
         <v>387</v>
-      </c>
-      <c r="D12" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>384</v>
+      </c>
+      <c r="B14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C14" t="s">
         <v>386</v>
       </c>
-      <c r="B14" t="s">
-        <v>395</v>
-      </c>
-      <c r="C14" t="s">
-        <v>388</v>
-      </c>
       <c r="D14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B15" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B16" t="s">
+        <v>392</v>
+      </c>
+      <c r="C16" t="s">
         <v>394</v>
       </c>
-      <c r="C16" t="s">
-        <v>396</v>
-      </c>
       <c r="D16" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B18" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C18" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D18" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B19" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to css, html, and javascript
Updated css file and html to be cleaner. Pulled two long sections of code out of the html and created separate js scripts called at the bottom. Also added a timer to the initial draw map to make sure the function does not try to run before the data are loaded.
</commit_message>
<xml_diff>
--- a/deploy/nc-water-supply/data/pcp/ncsu_api_locations.xlsx
+++ b/deploy/nc-water-supply/data/pcp/ncsu_api_locations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lap19\Documents\GitHub\TriangleWaterSupplyDashboard\deploy\nc-water-supply\data\pcp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lap19\Documents\Internet of Water\Pilots\NC\NC Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="408">
   <si>
     <t>B Everett Jordan Dam</t>
   </si>
@@ -1102,6 +1102,12 @@
   </si>
   <si>
     <t>actual start day: 11/1/1871</t>
+  </si>
+  <si>
+    <t>actual start date: 12/1/1870</t>
+  </si>
+  <si>
+    <t>actual start date: 1/1/1887</t>
   </si>
   <si>
     <t>actual start date: 1/15/1892</t>
@@ -1586,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29:L87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1603,6 @@
     <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1608,7 +1613,7 @@
         <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>87</v>
@@ -1646,7 +1651,7 @@
         <v>310750</v>
       </c>
       <c r="C2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1681,7 +1686,7 @@
         <v>311429</v>
       </c>
       <c r="C3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -1716,7 +1721,7 @@
         <v>311515</v>
       </c>
       <c r="C4" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -1751,7 +1756,7 @@
         <v>311677</v>
       </c>
       <c r="C5" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1789,7 +1794,7 @@
         <v>311700</v>
       </c>
       <c r="C6" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -1824,7 +1829,7 @@
         <v>311881</v>
       </c>
       <c r="C7" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -1859,7 +1864,7 @@
         <v>312500</v>
       </c>
       <c r="C8" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -1894,7 +1899,7 @@
         <v>312517</v>
       </c>
       <c r="C9" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -1929,7 +1934,7 @@
         <v>313017</v>
       </c>
       <c r="C10" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -1967,7 +1972,7 @@
         <v>313555</v>
       </c>
       <c r="C11" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -2002,7 +2007,7 @@
         <v>313630</v>
       </c>
       <c r="C12" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -2037,7 +2042,7 @@
         <v>313625</v>
       </c>
       <c r="C13" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -2072,7 +2077,7 @@
         <v>313919</v>
       </c>
       <c r="C14" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -2107,7 +2112,7 @@
         <v>314063</v>
       </c>
       <c r="C15" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -2142,7 +2147,7 @@
         <v>314471</v>
       </c>
       <c r="C16" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -2169,7 +2174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2177,7 +2182,7 @@
         <v>314987</v>
       </c>
       <c r="C17" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -2204,7 +2209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2212,7 +2217,7 @@
         <v>315820</v>
       </c>
       <c r="C18" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -2239,7 +2244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>315930</v>
       </c>
       <c r="C19" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
@@ -2274,7 +2279,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>316122</v>
       </c>
       <c r="C20" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
@@ -2309,7 +2314,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2317,7 +2322,7 @@
         <v>317097</v>
       </c>
       <c r="C21" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -2344,7 +2349,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>316422</v>
       </c>
       <c r="C22" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -2379,7 +2384,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2387,7 +2392,7 @@
         <v>317656</v>
       </c>
       <c r="C23" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -2414,7 +2419,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2422,7 +2427,7 @@
         <v>317924</v>
       </c>
       <c r="C24" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
@@ -2449,7 +2454,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>319026</v>
       </c>
       <c r="C25" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
@@ -2484,7 +2489,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -2492,7 +2497,7 @@
         <v>319467</v>
       </c>
       <c r="C26" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
@@ -2519,7 +2524,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>319461</v>
       </c>
       <c r="C27" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
@@ -2554,7 +2559,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -2562,7 +2567,7 @@
         <v>319457</v>
       </c>
       <c r="C28" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
@@ -2589,7 +2594,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>99</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>100</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>131</v>
@@ -2623,11 +2628,12 @@
       <c r="K29" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="L29" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L29" s="3"/>
+      <c r="M29" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>101</v>
       </c>
@@ -2635,7 +2641,7 @@
         <v>102</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>131</v>
@@ -2661,11 +2667,12 @@
       <c r="K30" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L30" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L30" s="3"/>
+      <c r="M30" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -2673,7 +2680,7 @@
         <v>106</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>131</v>
@@ -2699,11 +2706,12 @@
       <c r="K31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L31" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L31" s="3"/>
+      <c r="M31" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>109</v>
       </c>
@@ -2711,7 +2719,7 @@
         <v>110</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>131</v>
@@ -2737,11 +2745,12 @@
       <c r="K32" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L32" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L32" s="3"/>
+      <c r="M32" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>112</v>
       </c>
@@ -2749,7 +2758,7 @@
         <v>113</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>131</v>
@@ -2775,11 +2784,12 @@
       <c r="K33" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L33" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L33" s="3"/>
+      <c r="M33" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>115</v>
       </c>
@@ -2787,7 +2797,7 @@
         <v>116</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>131</v>
@@ -2813,11 +2823,12 @@
       <c r="K34" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L34" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L34" s="3"/>
+      <c r="M34" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>117</v>
       </c>
@@ -2825,7 +2836,7 @@
         <v>118</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>131</v>
@@ -2851,11 +2862,12 @@
       <c r="K35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="L35" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L35" s="3"/>
+      <c r="M35" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>120</v>
       </c>
@@ -2863,7 +2875,7 @@
         <v>121</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>131</v>
@@ -2889,11 +2901,12 @@
       <c r="K36" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L36" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L36" s="3"/>
+      <c r="M36" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>122</v>
       </c>
@@ -2901,7 +2914,7 @@
         <v>123</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>131</v>
@@ -2927,11 +2940,12 @@
       <c r="K37" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="L37" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L37" s="3"/>
+      <c r="M37" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>124</v>
       </c>
@@ -2939,7 +2953,7 @@
         <v>125</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>131</v>
@@ -2965,11 +2979,12 @@
       <c r="K38" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="L38" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L38" s="3"/>
+      <c r="M38" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>126</v>
       </c>
@@ -2977,7 +2992,7 @@
         <v>127</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>131</v>
@@ -3003,11 +3018,12 @@
       <c r="K39" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="L39" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L39" s="3"/>
+      <c r="M39" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>128</v>
       </c>
@@ -3015,7 +3031,7 @@
         <v>129</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>131</v>
@@ -3041,11 +3057,12 @@
       <c r="K40" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L40" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L40" s="3"/>
+      <c r="M40" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>144</v>
       </c>
@@ -3053,7 +3070,7 @@
         <v>145</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>146</v>
@@ -3079,11 +3096,12 @@
       <c r="K41" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L41" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L41" s="3"/>
+      <c r="M41" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>149</v>
       </c>
@@ -3091,7 +3109,7 @@
         <v>150</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>146</v>
@@ -3117,11 +3135,12 @@
       <c r="K42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L42" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L42" s="3"/>
+      <c r="M42" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>152</v>
       </c>
@@ -3129,7 +3148,7 @@
         <v>153</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>146</v>
@@ -3155,11 +3174,12 @@
       <c r="K43" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="L43" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L43" s="3"/>
+      <c r="M43" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>155</v>
       </c>
@@ -3167,7 +3187,7 @@
         <v>156</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>146</v>
@@ -3193,11 +3213,12 @@
       <c r="K44" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L44" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L44" s="3"/>
+      <c r="M44" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>158</v>
       </c>
@@ -3205,7 +3226,7 @@
         <v>2098197</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>203</v>
@@ -3231,11 +3252,12 @@
       <c r="K45" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="L45" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L45" s="5"/>
+      <c r="M45" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>29</v>
       </c>
@@ -3243,7 +3265,7 @@
         <v>159</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>205</v>
@@ -3269,11 +3291,12 @@
       <c r="K46" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L46" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L46" s="3"/>
+      <c r="M46" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>160</v>
       </c>
@@ -3281,7 +3304,7 @@
         <v>161</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>207</v>
@@ -3307,11 +3330,12 @@
       <c r="K47" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L47" s="5"/>
+      <c r="M47" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>163</v>
       </c>
@@ -3319,7 +3343,7 @@
         <v>164</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>209</v>
@@ -3345,11 +3369,12 @@
       <c r="K48" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L48" s="5"/>
+      <c r="M48" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>165</v>
       </c>
@@ -3357,7 +3382,7 @@
         <v>166</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>209</v>
@@ -3384,10 +3409,13 @@
         <v>211</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>167</v>
       </c>
@@ -3395,7 +3423,7 @@
         <v>168</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>212</v>
@@ -3421,11 +3449,12 @@
       <c r="K50" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L50" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L50" s="5"/>
+      <c r="M50" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>169</v>
       </c>
@@ -3433,7 +3462,7 @@
         <v>170</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>212</v>
@@ -3459,11 +3488,12 @@
       <c r="K51" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="L51" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L51" s="5"/>
+      <c r="M51" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>130</v>
       </c>
@@ -3471,7 +3501,7 @@
         <v>171</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>212</v>
@@ -3497,11 +3527,12 @@
       <c r="K52" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="L52" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L52" s="5"/>
+      <c r="M52" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>172</v>
       </c>
@@ -3509,7 +3540,7 @@
         <v>173</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>212</v>
@@ -3535,11 +3566,12 @@
       <c r="K53" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L53" s="5"/>
+      <c r="M53" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>175</v>
       </c>
@@ -3547,7 +3579,7 @@
         <v>176</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>212</v>
@@ -3573,11 +3605,12 @@
       <c r="K54" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="L54" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L54" s="5"/>
+      <c r="M54" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>178</v>
       </c>
@@ -3585,7 +3618,7 @@
         <v>179</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>212</v>
@@ -3611,11 +3644,12 @@
       <c r="K55" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="L55" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L55" s="5"/>
+      <c r="M55" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>181</v>
       </c>
@@ -3623,7 +3657,7 @@
         <v>182</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>212</v>
@@ -3649,11 +3683,12 @@
       <c r="K56" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="L56" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L56" s="5"/>
+      <c r="M56" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>183</v>
       </c>
@@ -3661,7 +3696,7 @@
         <v>184</v>
       </c>
       <c r="C57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D57" t="s">
         <v>220</v>
@@ -3688,7 +3723,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>186</v>
       </c>
@@ -3696,7 +3731,7 @@
         <v>187</v>
       </c>
       <c r="C58" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D58" t="s">
         <v>220</v>
@@ -3723,7 +3758,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>188</v>
       </c>
@@ -3731,7 +3766,7 @@
         <v>189</v>
       </c>
       <c r="C59" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D59" t="s">
         <v>220</v>
@@ -3758,7 +3793,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>191</v>
       </c>
@@ -3766,7 +3801,7 @@
         <v>192</v>
       </c>
       <c r="C60" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D60" t="s">
         <v>220</v>
@@ -3793,7 +3828,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>193</v>
       </c>
@@ -3801,7 +3836,7 @@
         <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D61" t="s">
         <v>220</v>
@@ -3828,7 +3863,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>195</v>
       </c>
@@ -3836,7 +3871,7 @@
         <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D62" t="s">
         <v>220</v>
@@ -3863,7 +3898,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -3871,7 +3906,7 @@
         <v>198</v>
       </c>
       <c r="C63" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D63" t="s">
         <v>220</v>
@@ -3898,7 +3933,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>201</v>
       </c>
@@ -3906,7 +3941,7 @@
         <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D64" t="s">
         <v>220</v>
@@ -3933,7 +3968,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>231</v>
       </c>
@@ -3941,7 +3976,7 @@
         <v>232</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>207</v>
@@ -3967,11 +4002,12 @@
       <c r="K65" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="L65" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L65" s="5"/>
+      <c r="M65" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>234</v>
       </c>
@@ -3979,7 +4015,7 @@
         <v>235</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>209</v>
@@ -4006,10 +4042,13 @@
         <v>237</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>238</v>
       </c>
@@ -4017,7 +4056,7 @@
         <v>239</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>212</v>
@@ -4043,11 +4082,12 @@
       <c r="K67" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="L67" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L67" s="5"/>
+      <c r="M67" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>243</v>
       </c>
@@ -4055,7 +4095,7 @@
         <v>244</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>212</v>
@@ -4081,11 +4121,12 @@
       <c r="K68" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="L68" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L68" s="5"/>
+      <c r="M68" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>247</v>
       </c>
@@ -4093,7 +4134,7 @@
         <v>248</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>249</v>
@@ -4119,11 +4160,12 @@
       <c r="K69" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="L69" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L69" s="3"/>
+      <c r="M69" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>251</v>
       </c>
@@ -4131,7 +4173,7 @@
         <v>252</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>249</v>
@@ -4157,11 +4199,12 @@
       <c r="K70" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="L70" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L70" s="3"/>
+      <c r="M70" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>254</v>
       </c>
@@ -4169,7 +4212,7 @@
         <v>255</v>
       </c>
       <c r="C71" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D71" t="s">
         <v>220</v>
@@ -4196,7 +4239,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>259</v>
       </c>
@@ -4204,7 +4247,7 @@
         <v>260</v>
       </c>
       <c r="C72" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D72" t="s">
         <v>220</v>
@@ -4231,7 +4274,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>264</v>
       </c>
@@ -4239,7 +4282,7 @@
         <v>265</v>
       </c>
       <c r="C73" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D73" t="s">
         <v>220</v>
@@ -4266,7 +4309,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>267</v>
       </c>
@@ -4274,7 +4317,7 @@
         <v>268</v>
       </c>
       <c r="C74" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D74" t="s">
         <v>220</v>
@@ -4301,7 +4344,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>272</v>
       </c>
@@ -4309,7 +4352,7 @@
         <v>273</v>
       </c>
       <c r="C75" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D75" t="s">
         <v>220</v>
@@ -4336,7 +4379,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>275</v>
       </c>
@@ -4344,7 +4387,7 @@
         <v>276</v>
       </c>
       <c r="C76" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D76" t="s">
         <v>220</v>
@@ -4371,7 +4414,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -4379,7 +4422,7 @@
         <v>279</v>
       </c>
       <c r="C77" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D77" t="s">
         <v>220</v>
@@ -4406,7 +4449,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>281</v>
       </c>
@@ -4414,7 +4457,7 @@
         <v>282</v>
       </c>
       <c r="C78" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D78" t="s">
         <v>220</v>
@@ -4441,7 +4484,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>284</v>
       </c>
@@ -4449,7 +4492,7 @@
         <v>285</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>146</v>
@@ -4475,11 +4518,12 @@
       <c r="K79" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="L79" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L79" s="3"/>
+      <c r="M79" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>287</v>
       </c>
@@ -4487,7 +4531,7 @@
         <v>288</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>146</v>
@@ -4513,11 +4557,12 @@
       <c r="K80" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="L80" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L80" s="3"/>
+      <c r="M80" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>290</v>
       </c>
@@ -4525,7 +4570,7 @@
         <v>291</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>131</v>
@@ -4551,11 +4596,12 @@
       <c r="K81" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="L81" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L81" s="3"/>
+      <c r="M81" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>294</v>
       </c>
@@ -4563,7 +4609,7 @@
         <v>295</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>131</v>
@@ -4589,11 +4635,12 @@
       <c r="K82" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="L82" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L82" s="3"/>
+      <c r="M82" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>297</v>
       </c>
@@ -4601,7 +4648,7 @@
         <v>298</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>131</v>
@@ -4627,11 +4674,12 @@
       <c r="K83" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="L83" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L83" s="3"/>
+      <c r="M83" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>301</v>
       </c>
@@ -4639,7 +4687,7 @@
         <v>302</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>131</v>
@@ -4665,11 +4713,12 @@
       <c r="K84" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="L84" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L84" s="3"/>
+      <c r="M84" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>306</v>
       </c>
@@ -4677,7 +4726,7 @@
         <v>307</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>131</v>
@@ -4703,11 +4752,12 @@
       <c r="K85" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="L85" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L85" s="3"/>
+      <c r="M85" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>311</v>
       </c>
@@ -4715,7 +4765,7 @@
         <v>312</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>131</v>
@@ -4741,11 +4791,12 @@
       <c r="K86" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="L86" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L86" s="3"/>
+      <c r="M86" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>314</v>
       </c>
@@ -4753,7 +4804,7 @@
         <v>315</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>131</v>
@@ -4779,11 +4830,12 @@
       <c r="K87" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="L87" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L87" s="3"/>
+      <c r="M87" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>64</v>
       </c>
@@ -4791,7 +4843,7 @@
         <v>310212</v>
       </c>
       <c r="C88" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
@@ -4818,7 +4870,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>318</v>
       </c>
@@ -4826,7 +4878,7 @@
         <v>311535</v>
       </c>
       <c r="C89" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D89" t="s">
         <v>1</v>
@@ -4853,7 +4905,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>320</v>
       </c>
@@ -4861,7 +4913,7 @@
         <v>311817</v>
       </c>
       <c r="C90" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
@@ -4888,7 +4940,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>322</v>
       </c>
@@ -4896,7 +4948,7 @@
         <v>311820</v>
       </c>
       <c r="C91" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
@@ -4923,7 +4975,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>231</v>
       </c>
@@ -4931,7 +4983,7 @@
         <v>312993</v>
       </c>
       <c r="C92" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
@@ -4958,7 +5010,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>326</v>
       </c>
@@ -4966,7 +5018,7 @@
         <v>313238</v>
       </c>
       <c r="C93" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
@@ -4993,7 +5045,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>328</v>
       </c>
@@ -5001,7 +5053,7 @@
         <v>313503</v>
       </c>
       <c r="C94" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D94" t="s">
         <v>1</v>
@@ -5028,7 +5080,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>330</v>
       </c>
@@ -5036,7 +5088,7 @@
         <v>314689</v>
       </c>
       <c r="C95" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D95" t="s">
         <v>1</v>
@@ -5063,7 +5115,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>332</v>
       </c>
@@ -5071,7 +5123,7 @@
         <v>316108</v>
       </c>
       <c r="C96" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
@@ -5106,7 +5158,7 @@
         <v>316676</v>
       </c>
       <c r="C97" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D97" t="s">
         <v>1</v>
@@ -5141,7 +5193,7 @@
         <v>317069</v>
       </c>
       <c r="C98" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D98" t="s">
         <v>1</v>
@@ -5176,7 +5228,7 @@
         <v>317079</v>
       </c>
       <c r="C99" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D99" t="s">
         <v>1</v>
@@ -5203,7 +5255,7 @@
         <v>341</v>
       </c>
       <c r="L99" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
@@ -5214,7 +5266,7 @@
         <v>317170</v>
       </c>
       <c r="C100" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D100" t="s">
         <v>1</v>
@@ -5249,7 +5301,7 @@
         <v>317516</v>
       </c>
       <c r="C101" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D101" t="s">
         <v>1</v>
@@ -5276,7 +5328,7 @@
         <v>346</v>
       </c>
       <c r="L101" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
@@ -5287,7 +5339,7 @@
         <v>317994</v>
       </c>
       <c r="C102" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
@@ -5314,7 +5366,7 @@
         <v>347</v>
       </c>
       <c r="L102" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
@@ -5325,7 +5377,7 @@
         <v>318066</v>
       </c>
       <c r="C103" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
@@ -5360,7 +5412,7 @@
         <v>319476</v>
       </c>
       <c r="C104" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D104" t="s">
         <v>1</v>
@@ -5409,268 +5461,268 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B7" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C7" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D7" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C8" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D8" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C9" t="s">
         <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B10" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B11" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C11" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D11" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B12" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C12" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D12" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B13" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C13" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D13" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B14" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C14" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D14" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B15" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C15" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D15" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B16" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C16" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D16" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B17" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C17" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D17" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B18" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C18" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D18" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B19" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C19" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D19" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>